<commit_message>
modify and delete test working but not writing to excel file
</commit_message>
<xml_diff>
--- a/part_c/test_results.xlsx
+++ b/part_c/test_results.xlsx
@@ -479,33 +479,33 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>54.61</v>
+      </c>
       <c r="C2">
-        <v>23.74</v>
-      </c>
-      <c r="E2">
-        <v>13.74</v>
+        <v>14.78</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>53.02</v>
+      </c>
       <c r="C3">
-        <v>17.52</v>
-      </c>
-      <c r="E3">
-        <v>11.88</v>
+        <v>14.07</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>47.46</v>
+      </c>
       <c r="C4">
-        <v>22.34</v>
-      </c>
-      <c r="E4">
-        <v>12.7</v>
+        <v>11.78</v>
       </c>
     </row>
   </sheetData>
@@ -560,33 +560,33 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>38.43</v>
+      </c>
       <c r="C2">
-        <v>11.92</v>
-      </c>
-      <c r="E2">
-        <v>8.210000000000001</v>
+        <v>13.97</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>35.42</v>
+      </c>
       <c r="C3">
-        <v>11.54</v>
-      </c>
-      <c r="E3">
-        <v>8.67</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>28.9</v>
+      </c>
       <c r="C4">
-        <v>9.890000000000001</v>
-      </c>
-      <c r="E4">
-        <v>13.65</v>
+        <v>10.11</v>
       </c>
     </row>
   </sheetData>
@@ -641,33 +641,33 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>31.67</v>
+      </c>
       <c r="C2">
-        <v>9.31</v>
-      </c>
-      <c r="E2">
-        <v>11.18</v>
+        <v>14.47</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>28.63</v>
+      </c>
       <c r="C3">
-        <v>8.18</v>
-      </c>
-      <c r="E3">
-        <v>12.08</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>34.05</v>
+      </c>
       <c r="C4">
-        <v>9.48</v>
-      </c>
-      <c r="E4">
-        <v>12.98</v>
+        <v>16.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>